<commit_message>
Cleaned up some blank space and a bigger FleetResParam.xlsx
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>NUM_AIRCRAFT</t>
   </si>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>SLEPspots</t>
-  </si>
-  <si>
-    <t>testlist</t>
-  </si>
-  <si>
-    <t>{'l':1, 'k':2}</t>
   </si>
 </sst>
 </file>
@@ -398,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,16 +452,13 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>80</v>
@@ -485,7 +476,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
-        <v>200</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I2">
         <v>7000</v>
@@ -512,18 +504,15 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>4</v>
-      </c>
-      <c r="R2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>80</v>
@@ -541,10 +530,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H3">
-        <v>500</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I3">
-        <v>6800</v>
+        <v>7000</v>
       </c>
       <c r="J3">
         <v>720</v>
@@ -568,18 +558,15 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>80</v>
@@ -597,10 +584,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H4">
-        <v>2000</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I4">
-        <v>6600</v>
+        <v>7000</v>
       </c>
       <c r="J4">
         <v>720</v>
@@ -624,10 +612,709 @@
         <v>1</v>
       </c>
       <c r="Q4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>720</v>
+      </c>
+      <c r="G5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H17" si="0">24*365*50</f>
+        <v>438000</v>
+      </c>
+      <c r="I5">
+        <v>7000</v>
+      </c>
+      <c r="J5">
+        <v>720</v>
+      </c>
+      <c r="K5">
+        <v>240</v>
+      </c>
+      <c r="L5">
+        <v>360</v>
+      </c>
+      <c r="M5">
+        <v>720</v>
+      </c>
+      <c r="N5">
+        <v>480</v>
+      </c>
+      <c r="O5">
+        <v>240</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>4</v>
       </c>
-      <c r="R4" t="s">
-        <v>18</v>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>84684684</v>
+      </c>
+      <c r="F6">
+        <v>720</v>
+      </c>
+      <c r="G6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I6">
+        <v>7000</v>
+      </c>
+      <c r="J6">
+        <v>720</v>
+      </c>
+      <c r="K6">
+        <v>240</v>
+      </c>
+      <c r="L6">
+        <v>360</v>
+      </c>
+      <c r="M6">
+        <v>720</v>
+      </c>
+      <c r="N6">
+        <v>480</v>
+      </c>
+      <c r="O6">
+        <v>240</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>84684684</v>
+      </c>
+      <c r="F7">
+        <v>720</v>
+      </c>
+      <c r="G7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I7">
+        <v>7000</v>
+      </c>
+      <c r="J7">
+        <v>720</v>
+      </c>
+      <c r="K7">
+        <v>240</v>
+      </c>
+      <c r="L7">
+        <v>360</v>
+      </c>
+      <c r="M7">
+        <v>720</v>
+      </c>
+      <c r="N7">
+        <v>480</v>
+      </c>
+      <c r="O7">
+        <v>240</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>84684684</v>
+      </c>
+      <c r="F8">
+        <v>720</v>
+      </c>
+      <c r="G8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I8">
+        <v>7000</v>
+      </c>
+      <c r="J8">
+        <v>720</v>
+      </c>
+      <c r="K8">
+        <v>240</v>
+      </c>
+      <c r="L8">
+        <v>360</v>
+      </c>
+      <c r="M8">
+        <v>720</v>
+      </c>
+      <c r="N8">
+        <v>480</v>
+      </c>
+      <c r="O8">
+        <v>240</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>84684684</v>
+      </c>
+      <c r="F9">
+        <v>720</v>
+      </c>
+      <c r="G9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I9">
+        <v>7000</v>
+      </c>
+      <c r="J9">
+        <v>720</v>
+      </c>
+      <c r="K9">
+        <v>240</v>
+      </c>
+      <c r="L9">
+        <v>360</v>
+      </c>
+      <c r="M9">
+        <v>720</v>
+      </c>
+      <c r="N9">
+        <v>480</v>
+      </c>
+      <c r="O9">
+        <v>240</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>454648</v>
+      </c>
+      <c r="F10">
+        <v>720</v>
+      </c>
+      <c r="G10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I10">
+        <v>7000</v>
+      </c>
+      <c r="J10">
+        <v>720</v>
+      </c>
+      <c r="K10">
+        <v>240</v>
+      </c>
+      <c r="L10">
+        <v>360</v>
+      </c>
+      <c r="M10">
+        <v>720</v>
+      </c>
+      <c r="N10">
+        <v>480</v>
+      </c>
+      <c r="O10">
+        <v>240</v>
+      </c>
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>454648</v>
+      </c>
+      <c r="F11">
+        <v>720</v>
+      </c>
+      <c r="G11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I11">
+        <v>7000</v>
+      </c>
+      <c r="J11">
+        <v>720</v>
+      </c>
+      <c r="K11">
+        <v>240</v>
+      </c>
+      <c r="L11">
+        <v>360</v>
+      </c>
+      <c r="M11">
+        <v>720</v>
+      </c>
+      <c r="N11">
+        <v>480</v>
+      </c>
+      <c r="O11">
+        <v>240</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>454648</v>
+      </c>
+      <c r="F12">
+        <v>720</v>
+      </c>
+      <c r="G12">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I12">
+        <v>7000</v>
+      </c>
+      <c r="J12">
+        <v>720</v>
+      </c>
+      <c r="K12">
+        <v>240</v>
+      </c>
+      <c r="L12">
+        <v>360</v>
+      </c>
+      <c r="M12">
+        <v>720</v>
+      </c>
+      <c r="N12">
+        <v>480</v>
+      </c>
+      <c r="O12">
+        <v>240</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>80</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>454648</v>
+      </c>
+      <c r="F13">
+        <v>720</v>
+      </c>
+      <c r="G13">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I13">
+        <v>7000</v>
+      </c>
+      <c r="J13">
+        <v>720</v>
+      </c>
+      <c r="K13">
+        <v>240</v>
+      </c>
+      <c r="L13">
+        <v>360</v>
+      </c>
+      <c r="M13">
+        <v>720</v>
+      </c>
+      <c r="N13">
+        <v>480</v>
+      </c>
+      <c r="O13">
+        <v>240</v>
+      </c>
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>80</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>88989534</v>
+      </c>
+      <c r="F14">
+        <v>720</v>
+      </c>
+      <c r="G14">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I14">
+        <v>7000</v>
+      </c>
+      <c r="J14">
+        <v>720</v>
+      </c>
+      <c r="K14">
+        <v>240</v>
+      </c>
+      <c r="L14">
+        <v>360</v>
+      </c>
+      <c r="M14">
+        <v>720</v>
+      </c>
+      <c r="N14">
+        <v>480</v>
+      </c>
+      <c r="O14">
+        <v>240</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>80</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>88989534</v>
+      </c>
+      <c r="F15">
+        <v>720</v>
+      </c>
+      <c r="G15">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I15">
+        <v>7000</v>
+      </c>
+      <c r="J15">
+        <v>720</v>
+      </c>
+      <c r="K15">
+        <v>240</v>
+      </c>
+      <c r="L15">
+        <v>360</v>
+      </c>
+      <c r="M15">
+        <v>720</v>
+      </c>
+      <c r="N15">
+        <v>480</v>
+      </c>
+      <c r="O15">
+        <v>240</v>
+      </c>
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>88989534</v>
+      </c>
+      <c r="F16">
+        <v>720</v>
+      </c>
+      <c r="G16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I16">
+        <v>7000</v>
+      </c>
+      <c r="J16">
+        <v>720</v>
+      </c>
+      <c r="K16">
+        <v>240</v>
+      </c>
+      <c r="L16">
+        <v>360</v>
+      </c>
+      <c r="M16">
+        <v>720</v>
+      </c>
+      <c r="N16">
+        <v>480</v>
+      </c>
+      <c r="O16">
+        <v>240</v>
+      </c>
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>88989534</v>
+      </c>
+      <c r="F17">
+        <v>720</v>
+      </c>
+      <c r="G17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I17">
+        <v>7000</v>
+      </c>
+      <c r="J17">
+        <v>720</v>
+      </c>
+      <c r="K17">
+        <v>240</v>
+      </c>
+      <c r="L17">
+        <v>360</v>
+      </c>
+      <c r="M17">
+        <v>720</v>
+      </c>
+      <c r="N17">
+        <v>480</v>
+      </c>
+      <c r="O17">
+        <v>240</v>
+      </c>
+      <c r="P17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fleet resilience now has a hard coded number of runs. Each line in FleetResParam should be an individual experiment. Each run continues with the same seed. The seed is reset for each experiment, so we know they have the same random seed with different inputs. This way, I only need one random seed for the entire experiment.
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H3" sqref="H3:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,13 +455,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -476,8 +476,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
-        <f>24*365*50</f>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I2">
         <v>7000</v>
@@ -509,13 +508,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C3">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -530,8 +529,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H3">
-        <f>24*365*50</f>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I3">
         <v>7000</v>
@@ -558,18 +556,18 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -584,8 +582,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H4">
-        <f>24*365*50</f>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I4">
         <v>7000</v>
@@ -612,18 +609,18 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -638,8 +635,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H17" si="0">24*365*50</f>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I5">
         <v>7000</v>
@@ -666,24 +662,24 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>25</v>
       </c>
       <c r="E6">
-        <v>84684684</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>720</v>
@@ -692,8 +688,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I6">
         <v>7000</v>
@@ -725,19 +720,19 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C7">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>25</v>
       </c>
       <c r="E7">
-        <v>84684684</v>
+        <v>42</v>
       </c>
       <c r="F7">
         <v>720</v>
@@ -746,8 +741,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I7">
         <v>7000</v>
@@ -774,24 +768,24 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C8">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="E8">
-        <v>84684684</v>
+        <v>42</v>
       </c>
       <c r="F8">
         <v>720</v>
@@ -800,8 +794,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I8">
         <v>7000</v>
@@ -828,24 +821,24 @@
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C9">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>25</v>
       </c>
       <c r="E9">
-        <v>84684684</v>
+        <v>42</v>
       </c>
       <c r="F9">
         <v>720</v>
@@ -854,8 +847,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I9">
         <v>7000</v>
@@ -882,24 +874,24 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C10">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>25</v>
       </c>
       <c r="E10">
-        <v>454648</v>
+        <v>42</v>
       </c>
       <c r="F10">
         <v>720</v>
@@ -908,8 +900,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I10">
         <v>7000</v>
@@ -941,19 +932,19 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C11">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>25</v>
       </c>
       <c r="E11">
-        <v>454648</v>
+        <v>42</v>
       </c>
       <c r="F11">
         <v>720</v>
@@ -962,8 +953,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I11">
         <v>7000</v>
@@ -990,24 +980,24 @@
         <v>1</v>
       </c>
       <c r="Q11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C12">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>25</v>
       </c>
       <c r="E12">
-        <v>454648</v>
+        <v>42</v>
       </c>
       <c r="F12">
         <v>720</v>
@@ -1016,8 +1006,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I12">
         <v>7000</v>
@@ -1044,24 +1033,24 @@
         <v>1</v>
       </c>
       <c r="Q12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>25</v>
       </c>
       <c r="E13">
-        <v>454648</v>
+        <v>42</v>
       </c>
       <c r="F13">
         <v>720</v>
@@ -1070,8 +1059,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I13">
         <v>7000</v>
@@ -1098,24 +1086,24 @@
         <v>1</v>
       </c>
       <c r="Q13">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C14">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>25</v>
       </c>
       <c r="E14">
-        <v>88989534</v>
+        <v>42</v>
       </c>
       <c r="F14">
         <v>720</v>
@@ -1124,8 +1112,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I14">
         <v>7000</v>
@@ -1157,19 +1144,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B15">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C15">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>25</v>
       </c>
       <c r="E15">
-        <v>88989534</v>
+        <v>42</v>
       </c>
       <c r="F15">
         <v>720</v>
@@ -1178,8 +1165,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I15">
         <v>7000</v>
@@ -1206,24 +1192,24 @@
         <v>1</v>
       </c>
       <c r="Q15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C16">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>25</v>
       </c>
       <c r="E16">
-        <v>88989534</v>
+        <v>42</v>
       </c>
       <c r="F16">
         <v>720</v>
@@ -1232,8 +1218,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I16">
         <v>7000</v>
@@ -1260,24 +1245,24 @@
         <v>1</v>
       </c>
       <c r="Q16">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C17">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>25</v>
       </c>
       <c r="E17">
-        <v>88989534</v>
+        <v>42</v>
       </c>
       <c r="F17">
         <v>720</v>
@@ -1286,8 +1271,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <v>4380</v>
       </c>
       <c r="I17">
         <v>7000</v>
@@ -1314,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="Q17">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A reasonable aggregation tool. an experiment. Let's seen what we can do.
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanurn1\Documents\Resilience\Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a35891ba506d4b9/PhD Work/Dissertation/Programming/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{D2D0288C-312E-4C79-9FDE-29127E4D8C98}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="11235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>NUM_AIRCRAFT</t>
   </si>
@@ -75,12 +81,21 @@
   </si>
   <si>
     <t>SLEPspots</t>
+  </si>
+  <si>
+    <t>addHours</t>
+  </si>
+  <si>
+    <t>Stagger</t>
+  </si>
+  <si>
+    <t>TTR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,16 +406,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H17"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +467,17 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50</v>
       </c>
@@ -476,7 +500,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I2">
         <v>7000</v>
@@ -503,10 +528,20 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>14400</v>
+      </c>
+      <c r="T2">
+        <f>24*30*9</f>
+        <v>6480</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -529,7 +564,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H3">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I3">
         <v>7000</v>
@@ -556,10 +592,20 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>10800</v>
+      </c>
+      <c r="T3">
+        <f>24*30*6</f>
+        <v>4320</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -582,7 +628,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H4">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I4">
         <v>7000</v>
@@ -609,10 +656,20 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>14400</v>
+      </c>
+      <c r="T4">
+        <f>24*30*9</f>
+        <v>6480</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -635,7 +692,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H5">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I5">
         <v>7000</v>
@@ -662,10 +720,20 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>10800</v>
+      </c>
+      <c r="T5">
+        <f>24*30*6</f>
+        <v>4320</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -688,7 +756,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H6">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I6">
         <v>7000</v>
@@ -715,10 +784,20 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>14400</v>
+      </c>
+      <c r="T6">
+        <f>24*30*9</f>
+        <v>6480</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -741,7 +820,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H7">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I7">
         <v>7000</v>
@@ -768,10 +848,20 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>10800</v>
+      </c>
+      <c r="T7">
+        <f>24*30*6</f>
+        <v>4320</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
@@ -794,7 +884,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H8">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I8">
         <v>7000</v>
@@ -821,10 +912,20 @@
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>14400</v>
+      </c>
+      <c r="T8">
+        <f>24*30*9</f>
+        <v>6480</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
@@ -847,7 +948,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H9">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I9">
         <v>7000</v>
@@ -874,10 +976,20 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>10800</v>
+      </c>
+      <c r="T9">
+        <f>24*30*6</f>
+        <v>4320</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -900,7 +1012,8 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H10">
-        <v>4380</v>
+        <f>24*365*50</f>
+        <v>438000</v>
       </c>
       <c r="I10">
         <v>7000</v>
@@ -924,381 +1037,20 @@
         <v>240</v>
       </c>
       <c r="P10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>50</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11">
-        <v>40</v>
-      </c>
-      <c r="D11">
-        <v>25</v>
-      </c>
-      <c r="E11">
-        <v>42</v>
-      </c>
-      <c r="F11">
-        <v>720</v>
-      </c>
-      <c r="G11">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H11">
-        <v>4380</v>
-      </c>
-      <c r="I11">
-        <v>7000</v>
-      </c>
-      <c r="J11">
-        <v>720</v>
-      </c>
-      <c r="K11">
-        <v>240</v>
-      </c>
-      <c r="L11">
-        <v>360</v>
-      </c>
-      <c r="M11">
-        <v>720</v>
-      </c>
-      <c r="N11">
-        <v>480</v>
-      </c>
-      <c r="O11">
-        <v>240</v>
-      </c>
-      <c r="P11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>25</v>
-      </c>
-      <c r="E12">
-        <v>42</v>
-      </c>
-      <c r="F12">
-        <v>720</v>
-      </c>
-      <c r="G12">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H12">
-        <v>4380</v>
-      </c>
-      <c r="I12">
-        <v>7000</v>
-      </c>
-      <c r="J12">
-        <v>720</v>
-      </c>
-      <c r="K12">
-        <v>240</v>
-      </c>
-      <c r="L12">
-        <v>360</v>
-      </c>
-      <c r="M12">
-        <v>720</v>
-      </c>
-      <c r="N12">
-        <v>480</v>
-      </c>
-      <c r="O12">
-        <v>240</v>
-      </c>
-      <c r="P12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>40</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-      <c r="E13">
-        <v>42</v>
-      </c>
-      <c r="F13">
-        <v>720</v>
-      </c>
-      <c r="G13">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H13">
-        <v>4380</v>
-      </c>
-      <c r="I13">
-        <v>7000</v>
-      </c>
-      <c r="J13">
-        <v>720</v>
-      </c>
-      <c r="K13">
-        <v>240</v>
-      </c>
-      <c r="L13">
-        <v>360</v>
-      </c>
-      <c r="M13">
-        <v>720</v>
-      </c>
-      <c r="N13">
-        <v>480</v>
-      </c>
-      <c r="O13">
-        <v>240</v>
-      </c>
-      <c r="P13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>50</v>
-      </c>
-      <c r="B14">
-        <v>50</v>
-      </c>
-      <c r="C14">
-        <v>40</v>
-      </c>
-      <c r="D14">
-        <v>25</v>
-      </c>
-      <c r="E14">
-        <v>42</v>
-      </c>
-      <c r="F14">
-        <v>720</v>
-      </c>
-      <c r="G14">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H14">
-        <v>4380</v>
-      </c>
-      <c r="I14">
-        <v>7000</v>
-      </c>
-      <c r="J14">
-        <v>720</v>
-      </c>
-      <c r="K14">
-        <v>240</v>
-      </c>
-      <c r="L14">
-        <v>360</v>
-      </c>
-      <c r="M14">
-        <v>720</v>
-      </c>
-      <c r="N14">
-        <v>480</v>
-      </c>
-      <c r="O14">
-        <v>240</v>
-      </c>
-      <c r="P14" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>50</v>
-      </c>
-      <c r="B15">
-        <v>50</v>
-      </c>
-      <c r="C15">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
-        <v>42</v>
-      </c>
-      <c r="F15">
-        <v>720</v>
-      </c>
-      <c r="G15">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H15">
-        <v>4380</v>
-      </c>
-      <c r="I15">
-        <v>7000</v>
-      </c>
-      <c r="J15">
-        <v>720</v>
-      </c>
-      <c r="K15">
-        <v>240</v>
-      </c>
-      <c r="L15">
-        <v>360</v>
-      </c>
-      <c r="M15">
-        <v>720</v>
-      </c>
-      <c r="N15">
-        <v>480</v>
-      </c>
-      <c r="O15">
-        <v>240</v>
-      </c>
-      <c r="P15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>50</v>
-      </c>
-      <c r="B16">
-        <v>50</v>
-      </c>
-      <c r="C16">
-        <v>40</v>
-      </c>
-      <c r="D16">
-        <v>25</v>
-      </c>
-      <c r="E16">
-        <v>42</v>
-      </c>
-      <c r="F16">
-        <v>720</v>
-      </c>
-      <c r="G16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H16">
-        <v>4380</v>
-      </c>
-      <c r="I16">
-        <v>7000</v>
-      </c>
-      <c r="J16">
-        <v>720</v>
-      </c>
-      <c r="K16">
-        <v>240</v>
-      </c>
-      <c r="L16">
-        <v>360</v>
-      </c>
-      <c r="M16">
-        <v>720</v>
-      </c>
-      <c r="N16">
-        <v>480</v>
-      </c>
-      <c r="O16">
-        <v>240</v>
-      </c>
-      <c r="P16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>50</v>
-      </c>
-      <c r="B17">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>40</v>
-      </c>
-      <c r="D17">
-        <v>25</v>
-      </c>
-      <c r="E17">
-        <v>42</v>
-      </c>
-      <c r="F17">
-        <v>720</v>
-      </c>
-      <c r="G17">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H17">
-        <v>4380</v>
-      </c>
-      <c r="I17">
-        <v>7000</v>
-      </c>
-      <c r="J17">
-        <v>720</v>
-      </c>
-      <c r="K17">
-        <v>240</v>
-      </c>
-      <c r="L17">
-        <v>360</v>
-      </c>
-      <c r="M17">
-        <v>720</v>
-      </c>
-      <c r="N17">
-        <v>480</v>
-      </c>
-      <c r="O17">
-        <v>240</v>
-      </c>
-      <c r="P17" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>10800</v>
+      </c>
+      <c r="T10">
+        <f>24*30*6</f>
+        <v>4320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a sundown program for further investigation. This .xslx provided the experiment
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a35891ba506d4b9/PhD Work/Dissertation/Programming/Metrics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PhD Work\Dissertation\Programming\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{D2D0288C-312E-4C79-9FDE-29127E4D8C98}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{06D52642-EB29-4AF8-A15B-1A0293D4E935}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>NUM_AIRCRAFT</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>TTR</t>
+  </si>
+  <si>
+    <t>sunDownDate</t>
+  </si>
+  <si>
+    <t>sunDownLength</t>
   </si>
 </sst>
 </file>
@@ -407,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,8 +482,14 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50</v>
       </c>
@@ -485,7 +497,7 @@
         <v>50</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -500,7 +512,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
-        <f>24*365*50</f>
+        <f t="shared" ref="H2:H16" si="0">24*365*50</f>
         <v>438000</v>
       </c>
       <c r="I2">
@@ -528,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
@@ -541,7 +553,7 @@
         <v>6480</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -549,7 +561,7 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -564,7 +576,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H3">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I3">
@@ -592,20 +604,20 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R3" t="b">
         <v>1</v>
       </c>
       <c r="S3">
-        <v>10800</v>
+        <v>14400</v>
       </c>
       <c r="T3">
-        <f>24*30*6</f>
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <f>24*30*9</f>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -613,7 +625,7 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -628,7 +640,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H4">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I4">
@@ -665,11 +677,11 @@
         <v>14400</v>
       </c>
       <c r="T4">
-        <f>24*30*9</f>
+        <f t="shared" ref="T4:T16" si="1">24*30*9</f>
         <v>6480</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -677,7 +689,7 @@
         <v>50</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -692,7 +704,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H5">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I5">
@@ -726,14 +738,14 @@
         <v>1</v>
       </c>
       <c r="S5">
-        <v>10800</v>
+        <v>14400</v>
       </c>
       <c r="T5">
-        <f>24*30*6</f>
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -741,7 +753,7 @@
         <v>50</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <v>25</v>
@@ -756,7 +768,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H6">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I6">
@@ -784,20 +796,20 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <v>14400</v>
       </c>
       <c r="T6">
-        <f>24*30*9</f>
+        <f t="shared" si="1"/>
         <v>6480</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -805,10 +817,10 @@
         <v>50</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>42</v>
@@ -820,7 +832,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H7">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I7">
@@ -848,20 +860,20 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>10800</v>
+        <v>14400</v>
       </c>
       <c r="T7">
-        <f>24*30*6</f>
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
@@ -869,10 +881,10 @@
         <v>50</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>42</v>
@@ -884,7 +896,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H8">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I8">
@@ -915,17 +927,17 @@
         <v>8</v>
       </c>
       <c r="R8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <v>14400</v>
       </c>
       <c r="T8">
-        <f>24*30*9</f>
+        <f t="shared" si="1"/>
         <v>6480</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
@@ -933,10 +945,10 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>42</v>
@@ -948,7 +960,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H9">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I9">
@@ -979,17 +991,17 @@
         <v>8</v>
       </c>
       <c r="R9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>10800</v>
+        <v>14400</v>
       </c>
       <c r="T9">
-        <f>24*30*6</f>
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -997,10 +1009,10 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E10">
         <v>42</v>
@@ -1012,7 +1024,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H10">
-        <f>24*365*50</f>
+        <f t="shared" si="0"/>
         <v>438000</v>
       </c>
       <c r="I10">
@@ -1037,20 +1049,404 @@
         <v>240</v>
       </c>
       <c r="P10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <v>10800</v>
+        <v>14400</v>
       </c>
       <c r="T10">
-        <f>24*30*6</f>
-        <v>4320</v>
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>90</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>720</v>
+      </c>
+      <c r="G11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I11">
+        <v>7000</v>
+      </c>
+      <c r="J11">
+        <v>720</v>
+      </c>
+      <c r="K11">
+        <v>240</v>
+      </c>
+      <c r="L11">
+        <v>360</v>
+      </c>
+      <c r="M11">
+        <v>720</v>
+      </c>
+      <c r="N11">
+        <v>480</v>
+      </c>
+      <c r="O11">
+        <v>240</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>14400</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>75</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>720</v>
+      </c>
+      <c r="G12">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I12">
+        <v>7000</v>
+      </c>
+      <c r="J12">
+        <v>720</v>
+      </c>
+      <c r="K12">
+        <v>240</v>
+      </c>
+      <c r="L12">
+        <v>360</v>
+      </c>
+      <c r="M12">
+        <v>720</v>
+      </c>
+      <c r="N12">
+        <v>480</v>
+      </c>
+      <c r="O12">
+        <v>240</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>8</v>
+      </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>14400</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>75</v>
+      </c>
+      <c r="E13">
+        <v>42</v>
+      </c>
+      <c r="F13">
+        <v>720</v>
+      </c>
+      <c r="G13">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I13">
+        <v>7000</v>
+      </c>
+      <c r="J13">
+        <v>720</v>
+      </c>
+      <c r="K13">
+        <v>240</v>
+      </c>
+      <c r="L13">
+        <v>360</v>
+      </c>
+      <c r="M13">
+        <v>720</v>
+      </c>
+      <c r="N13">
+        <v>480</v>
+      </c>
+      <c r="O13">
+        <v>240</v>
+      </c>
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>8</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>14400</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>75</v>
+      </c>
+      <c r="E14">
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <v>720</v>
+      </c>
+      <c r="G14">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I14">
+        <v>7000</v>
+      </c>
+      <c r="J14">
+        <v>720</v>
+      </c>
+      <c r="K14">
+        <v>240</v>
+      </c>
+      <c r="L14">
+        <v>360</v>
+      </c>
+      <c r="M14">
+        <v>720</v>
+      </c>
+      <c r="N14">
+        <v>480</v>
+      </c>
+      <c r="O14">
+        <v>240</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>8</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>14400</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>75</v>
+      </c>
+      <c r="E15">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>720</v>
+      </c>
+      <c r="G15">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I15">
+        <v>7000</v>
+      </c>
+      <c r="J15">
+        <v>720</v>
+      </c>
+      <c r="K15">
+        <v>240</v>
+      </c>
+      <c r="L15">
+        <v>360</v>
+      </c>
+      <c r="M15">
+        <v>720</v>
+      </c>
+      <c r="N15">
+        <v>480</v>
+      </c>
+      <c r="O15">
+        <v>240</v>
+      </c>
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>8</v>
+      </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>14400</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>90</v>
+      </c>
+      <c r="D16">
+        <v>75</v>
+      </c>
+      <c r="E16">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>720</v>
+      </c>
+      <c r="G16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="I16">
+        <v>7000</v>
+      </c>
+      <c r="J16">
+        <v>720</v>
+      </c>
+      <c r="K16">
+        <v>240</v>
+      </c>
+      <c r="L16">
+        <v>360</v>
+      </c>
+      <c r="M16">
+        <v>720</v>
+      </c>
+      <c r="N16">
+        <v>480</v>
+      </c>
+      <c r="O16">
+        <v>240</v>
+      </c>
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>8</v>
+      </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>14400</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>6480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Experiment with the SLEP lines fixed. I had put the variables in, but nothing was changing. That was fixed in the previous commit of the simulation.
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\PhD Work\Dissertation\Programming\Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a35891ba506d4b9/PhD Work/Dissertation/Programming/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{06D52642-EB29-4AF8-A15B-1A0293D4E935}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{8BB5E582-B83D-451C-B40C-8A9BD231F77A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>50</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -512,7 +512,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H16" si="0">24*365*50</f>
+        <f t="shared" ref="H2:H10" si="0">24*365*50</f>
         <v>438000</v>
       </c>
       <c r="I2">
@@ -540,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R2" t="b">
         <v>1</v>
@@ -552,6 +552,14 @@
         <f>24*30*9</f>
         <v>6480</v>
       </c>
+      <c r="U2">
+        <f>22*365*24</f>
+        <v>192720</v>
+      </c>
+      <c r="V2">
+        <f>5*365*24</f>
+        <v>43800</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -561,7 +569,7 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -604,17 +612,25 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R3" t="b">
         <v>1</v>
       </c>
       <c r="S3">
-        <v>14400</v>
+        <v>10800</v>
       </c>
       <c r="T3">
-        <f>24*30*9</f>
-        <v>6480</v>
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U3">
+        <f>22*365*24</f>
+        <v>192720</v>
+      </c>
+      <c r="V3">
+        <f>5*365*24</f>
+        <v>43800</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -625,7 +641,7 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -677,8 +693,16 @@
         <v>14400</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T16" si="1">24*30*9</f>
+        <f>24*30*9</f>
         <v>6480</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ref="U4:U10" si="1">22*365*24</f>
+        <v>192720</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V10" si="2">5*365*24</f>
+        <v>43800</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -689,7 +713,7 @@
         <v>50</v>
       </c>
       <c r="C5">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -738,11 +762,19 @@
         <v>1</v>
       </c>
       <c r="S5">
-        <v>14400</v>
+        <v>10800</v>
       </c>
       <c r="T5">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U5">
         <f t="shared" si="1"/>
-        <v>6480</v>
+        <v>192720</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="2"/>
+        <v>43800</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -753,7 +785,7 @@
         <v>50</v>
       </c>
       <c r="C6">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>25</v>
@@ -796,17 +828,25 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <v>14400</v>
       </c>
       <c r="T6">
+        <f>24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U6">
         <f t="shared" si="1"/>
-        <v>6480</v>
+        <v>192720</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>43800</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -817,10 +857,10 @@
         <v>50</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>42</v>
@@ -860,17 +900,25 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>14400</v>
+        <v>10800</v>
       </c>
       <c r="T7">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="1"/>
-        <v>6480</v>
+        <v>192720</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="2"/>
+        <v>43800</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -881,10 +929,10 @@
         <v>50</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <v>42</v>
@@ -927,14 +975,22 @@
         <v>8</v>
       </c>
       <c r="R8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <v>14400</v>
       </c>
       <c r="T8">
+        <f>24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U8">
         <f t="shared" si="1"/>
-        <v>6480</v>
+        <v>192720</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="2"/>
+        <v>43800</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -945,10 +1001,10 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>42</v>
@@ -991,14 +1047,22 @@
         <v>8</v>
       </c>
       <c r="R9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>14400</v>
+        <v>10800</v>
       </c>
       <c r="T9">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="1"/>
-        <v>6480</v>
+        <v>192720</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="2"/>
+        <v>43800</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1009,10 +1073,10 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E10">
         <v>42</v>
@@ -1049,404 +1113,28 @@
         <v>240</v>
       </c>
       <c r="P10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>14400</v>
+        <v>10800</v>
       </c>
       <c r="T10">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="1"/>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>50</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11">
-        <v>90</v>
-      </c>
-      <c r="D11">
-        <v>50</v>
-      </c>
-      <c r="E11">
-        <v>42</v>
-      </c>
-      <c r="F11">
-        <v>720</v>
-      </c>
-      <c r="G11">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-      <c r="I11">
-        <v>7000</v>
-      </c>
-      <c r="J11">
-        <v>720</v>
-      </c>
-      <c r="K11">
-        <v>240</v>
-      </c>
-      <c r="L11">
-        <v>360</v>
-      </c>
-      <c r="M11">
-        <v>720</v>
-      </c>
-      <c r="N11">
-        <v>480</v>
-      </c>
-      <c r="O11">
-        <v>240</v>
-      </c>
-      <c r="P11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>8</v>
-      </c>
-      <c r="R11" t="b">
-        <v>1</v>
-      </c>
-      <c r="S11">
-        <v>14400</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="1"/>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>75</v>
-      </c>
-      <c r="E12">
-        <v>42</v>
-      </c>
-      <c r="F12">
-        <v>720</v>
-      </c>
-      <c r="G12">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-      <c r="I12">
-        <v>7000</v>
-      </c>
-      <c r="J12">
-        <v>720</v>
-      </c>
-      <c r="K12">
-        <v>240</v>
-      </c>
-      <c r="L12">
-        <v>360</v>
-      </c>
-      <c r="M12">
-        <v>720</v>
-      </c>
-      <c r="N12">
-        <v>480</v>
-      </c>
-      <c r="O12">
-        <v>240</v>
-      </c>
-      <c r="P12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>8</v>
-      </c>
-      <c r="R12" t="b">
-        <v>1</v>
-      </c>
-      <c r="S12">
-        <v>14400</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="1"/>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>75</v>
-      </c>
-      <c r="E13">
-        <v>42</v>
-      </c>
-      <c r="F13">
-        <v>720</v>
-      </c>
-      <c r="G13">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-      <c r="I13">
-        <v>7000</v>
-      </c>
-      <c r="J13">
-        <v>720</v>
-      </c>
-      <c r="K13">
-        <v>240</v>
-      </c>
-      <c r="L13">
-        <v>360</v>
-      </c>
-      <c r="M13">
-        <v>720</v>
-      </c>
-      <c r="N13">
-        <v>480</v>
-      </c>
-      <c r="O13">
-        <v>240</v>
-      </c>
-      <c r="P13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>8</v>
-      </c>
-      <c r="R13" t="b">
-        <v>1</v>
-      </c>
-      <c r="S13">
-        <v>14400</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="1"/>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>50</v>
-      </c>
-      <c r="B14">
-        <v>50</v>
-      </c>
-      <c r="C14">
-        <v>50</v>
-      </c>
-      <c r="D14">
-        <v>75</v>
-      </c>
-      <c r="E14">
-        <v>42</v>
-      </c>
-      <c r="F14">
-        <v>720</v>
-      </c>
-      <c r="G14">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-      <c r="I14">
-        <v>7000</v>
-      </c>
-      <c r="J14">
-        <v>720</v>
-      </c>
-      <c r="K14">
-        <v>240</v>
-      </c>
-      <c r="L14">
-        <v>360</v>
-      </c>
-      <c r="M14">
-        <v>720</v>
-      </c>
-      <c r="N14">
-        <v>480</v>
-      </c>
-      <c r="O14">
-        <v>240</v>
-      </c>
-      <c r="P14" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>8</v>
-      </c>
-      <c r="R14" t="b">
-        <v>1</v>
-      </c>
-      <c r="S14">
-        <v>14400</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="1"/>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>50</v>
-      </c>
-      <c r="B15">
-        <v>50</v>
-      </c>
-      <c r="C15">
-        <v>70</v>
-      </c>
-      <c r="D15">
-        <v>75</v>
-      </c>
-      <c r="E15">
-        <v>42</v>
-      </c>
-      <c r="F15">
-        <v>720</v>
-      </c>
-      <c r="G15">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-      <c r="I15">
-        <v>7000</v>
-      </c>
-      <c r="J15">
-        <v>720</v>
-      </c>
-      <c r="K15">
-        <v>240</v>
-      </c>
-      <c r="L15">
-        <v>360</v>
-      </c>
-      <c r="M15">
-        <v>720</v>
-      </c>
-      <c r="N15">
-        <v>480</v>
-      </c>
-      <c r="O15">
-        <v>240</v>
-      </c>
-      <c r="P15" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>8</v>
-      </c>
-      <c r="R15" t="b">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>14400</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="1"/>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>50</v>
-      </c>
-      <c r="B16">
-        <v>50</v>
-      </c>
-      <c r="C16">
-        <v>90</v>
-      </c>
-      <c r="D16">
-        <v>75</v>
-      </c>
-      <c r="E16">
-        <v>42</v>
-      </c>
-      <c r="F16">
-        <v>720</v>
-      </c>
-      <c r="G16">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-      <c r="I16">
-        <v>7000</v>
-      </c>
-      <c r="J16">
-        <v>720</v>
-      </c>
-      <c r="K16">
-        <v>240</v>
-      </c>
-      <c r="L16">
-        <v>360</v>
-      </c>
-      <c r="M16">
-        <v>720</v>
-      </c>
-      <c r="N16">
-        <v>480</v>
-      </c>
-      <c r="O16">
-        <v>240</v>
-      </c>
-      <c r="P16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>8</v>
-      </c>
-      <c r="R16" t="b">
-        <v>1</v>
-      </c>
-      <c r="S16">
-        <v>14400</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="1"/>
-        <v>6480</v>
+        <v>192720</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>43800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready for runs for record.
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a35891ba506d4b9/PhD Work/Dissertation/Programming/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{8BB5E582-B83D-451C-B40C-8A9BD231F77A}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{F8F2510B-D2AB-4D5C-9A13-AB7A441E894C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>NUM_AIRCRAFT</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>sunDownLength</t>
+  </si>
+  <si>
+    <t>surgetime</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Base case no SLEP</t>
+  </si>
+  <si>
+    <t>Base SLEP case with no stagger</t>
   </si>
 </sst>
 </file>
@@ -413,15 +425,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="Q35" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="22" max="22" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +503,14 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50</v>
       </c>
@@ -512,20 +533,20 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H10" si="0">24*365*50</f>
+        <f>50*24*365</f>
         <v>438000</v>
       </c>
       <c r="I2">
         <v>7000</v>
       </c>
       <c r="J2">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="K2">
-        <v>240</v>
+        <v>30</v>
       </c>
       <c r="L2">
-        <v>360</v>
+        <v>40</v>
       </c>
       <c r="M2">
         <v>720</v>
@@ -537,31 +558,38 @@
         <v>240</v>
       </c>
       <c r="P2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>4</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>14400</v>
+        <v>10800</v>
       </c>
       <c r="T2">
-        <f>24*30*9</f>
-        <v>6480</v>
+        <f>24*30*6</f>
+        <v>4320</v>
       </c>
       <c r="U2">
-        <f>22*365*24</f>
-        <v>192720</v>
+        <f>50*365*24</f>
+        <v>438000</v>
       </c>
       <c r="V2">
         <f>5*365*24</f>
         <v>43800</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2">
+        <f t="shared" ref="W2:W18" si="0">50*365*24</f>
+        <v>438000</v>
+      </c>
+      <c r="X2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -584,20 +612,20 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f>50*24*365</f>
         <v>438000</v>
       </c>
       <c r="I3">
         <v>7000</v>
       </c>
       <c r="J3">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="K3">
-        <v>240</v>
+        <v>30</v>
       </c>
       <c r="L3">
-        <v>360</v>
+        <v>40</v>
       </c>
       <c r="M3">
         <v>720</v>
@@ -612,10 +640,10 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3" t="b">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
       </c>
       <c r="S3">
         <v>10800</v>
@@ -625,15 +653,22 @@
         <v>4320</v>
       </c>
       <c r="U3">
-        <f>22*365*24</f>
-        <v>192720</v>
+        <f>50*365*24</f>
+        <v>438000</v>
       </c>
       <c r="V3">
         <f>5*365*24</f>
         <v>43800</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W3">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+      <c r="X3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -656,56 +691,60 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H4">
+        <f t="shared" ref="H4:H27" si="1">50*24*365</f>
+        <v>438000</v>
+      </c>
+      <c r="I4">
+        <v>7000</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>40</v>
+      </c>
+      <c r="M4">
+        <v>720</v>
+      </c>
+      <c r="N4">
+        <v>480</v>
+      </c>
+      <c r="O4">
+        <v>240</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>0.5</v>
+      </c>
+      <c r="S4">
+        <v>10800</v>
+      </c>
+      <c r="T4">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U4">
+        <f>25*365*24</f>
+        <v>219000</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V27" si="2">5*365*24</f>
+        <v>43800</v>
+      </c>
+      <c r="W4">
         <f t="shared" si="0"/>
         <v>438000</v>
       </c>
-      <c r="I4">
-        <v>7000</v>
-      </c>
-      <c r="J4">
-        <v>720</v>
-      </c>
-      <c r="K4">
-        <v>240</v>
-      </c>
-      <c r="L4">
-        <v>360</v>
-      </c>
-      <c r="M4">
-        <v>720</v>
-      </c>
-      <c r="N4">
-        <v>480</v>
-      </c>
-      <c r="O4">
-        <v>240</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>8</v>
-      </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>14400</v>
-      </c>
-      <c r="T4">
-        <f>24*30*9</f>
-        <v>6480</v>
-      </c>
-      <c r="U4">
-        <f t="shared" ref="U4:U10" si="1">22*365*24</f>
-        <v>192720</v>
-      </c>
-      <c r="V4">
-        <f t="shared" ref="V4:V10" si="2">5*365*24</f>
-        <v>43800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -728,20 +767,20 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="I5">
         <v>7000</v>
       </c>
       <c r="J5">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="K5">
-        <v>240</v>
+        <v>30</v>
       </c>
       <c r="L5">
-        <v>360</v>
+        <v>40</v>
       </c>
       <c r="M5">
         <v>720</v>
@@ -758,8 +797,8 @@
       <c r="Q5">
         <v>8</v>
       </c>
-      <c r="R5" t="b">
-        <v>1</v>
+      <c r="R5">
+        <v>0.5</v>
       </c>
       <c r="S5">
         <v>10800</v>
@@ -769,15 +808,19 @@
         <v>4320</v>
       </c>
       <c r="U5">
-        <f t="shared" si="1"/>
-        <v>192720</v>
+        <f>30*365*24</f>
+        <v>262800</v>
       </c>
       <c r="V5">
         <f t="shared" si="2"/>
         <v>43800</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -800,128 +843,136 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H6">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I6">
+        <v>7000</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <v>30</v>
+      </c>
+      <c r="L6">
+        <v>40</v>
+      </c>
+      <c r="M6">
+        <v>720</v>
+      </c>
+      <c r="N6">
+        <v>480</v>
+      </c>
+      <c r="O6">
+        <v>240</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>8</v>
+      </c>
+      <c r="R6">
+        <v>0.5</v>
+      </c>
+      <c r="S6">
+        <v>10800</v>
+      </c>
+      <c r="T6">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U6">
+        <f>35*365*24</f>
+        <v>306600</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W6">
         <f t="shared" si="0"/>
         <v>438000</v>
       </c>
-      <c r="I6">
-        <v>7000</v>
-      </c>
-      <c r="J6">
-        <v>720</v>
-      </c>
-      <c r="K6">
-        <v>240</v>
-      </c>
-      <c r="L6">
-        <v>360</v>
-      </c>
-      <c r="M6">
-        <v>720</v>
-      </c>
-      <c r="N6">
-        <v>480</v>
-      </c>
-      <c r="O6">
-        <v>240</v>
-      </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>4</v>
-      </c>
-      <c r="R6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6">
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>720</v>
+      </c>
+      <c r="G7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I7">
+        <v>7000</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <v>30</v>
+      </c>
+      <c r="L7">
+        <v>40</v>
+      </c>
+      <c r="M7">
+        <v>720</v>
+      </c>
+      <c r="N7">
+        <v>480</v>
+      </c>
+      <c r="O7">
+        <v>240</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>8</v>
+      </c>
+      <c r="R7">
+        <v>0.5</v>
+      </c>
+      <c r="S7">
         <v>14400</v>
       </c>
-      <c r="T6">
+      <c r="T7">
         <f>24*30*9</f>
         <v>6480</v>
       </c>
-      <c r="U6">
-        <f t="shared" si="1"/>
-        <v>192720</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="2"/>
-        <v>43800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>50</v>
-      </c>
-      <c r="B7">
-        <v>50</v>
-      </c>
-      <c r="C7">
-        <v>40</v>
-      </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
-      <c r="E7">
-        <v>42</v>
-      </c>
-      <c r="F7">
-        <v>720</v>
-      </c>
-      <c r="G7">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-      <c r="I7">
-        <v>7000</v>
-      </c>
-      <c r="J7">
-        <v>720</v>
-      </c>
-      <c r="K7">
-        <v>240</v>
-      </c>
-      <c r="L7">
-        <v>360</v>
-      </c>
-      <c r="M7">
-        <v>720</v>
-      </c>
-      <c r="N7">
-        <v>480</v>
-      </c>
-      <c r="O7">
-        <v>240</v>
-      </c>
-      <c r="P7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>4</v>
-      </c>
-      <c r="R7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>10800</v>
-      </c>
-      <c r="T7">
-        <f>24*30*6</f>
-        <v>4320</v>
-      </c>
       <c r="U7">
-        <f t="shared" si="1"/>
-        <v>192720</v>
+        <f>25*365*24</f>
+        <v>219000</v>
       </c>
       <c r="V7">
         <f t="shared" si="2"/>
         <v>43800</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
@@ -944,20 +995,20 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="I8">
         <v>7000</v>
       </c>
       <c r="J8">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="K8">
-        <v>240</v>
+        <v>30</v>
       </c>
       <c r="L8">
-        <v>360</v>
+        <v>40</v>
       </c>
       <c r="M8">
         <v>720</v>
@@ -974,26 +1025,30 @@
       <c r="Q8">
         <v>8</v>
       </c>
-      <c r="R8" t="b">
-        <v>0</v>
+      <c r="R8">
+        <v>0.5</v>
       </c>
       <c r="S8">
         <v>14400</v>
       </c>
       <c r="T8">
-        <f>24*30*9</f>
+        <f t="shared" ref="T8:T9" si="3">24*30*9</f>
         <v>6480</v>
       </c>
       <c r="U8">
-        <f t="shared" si="1"/>
-        <v>192720</v>
+        <f>30*365*24</f>
+        <v>262800</v>
       </c>
       <c r="V8">
         <f t="shared" si="2"/>
         <v>43800</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W8">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
@@ -1016,20 +1071,20 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="I9">
         <v>7000</v>
       </c>
       <c r="J9">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="K9">
-        <v>240</v>
+        <v>30</v>
       </c>
       <c r="L9">
-        <v>360</v>
+        <v>40</v>
       </c>
       <c r="M9">
         <v>720</v>
@@ -1046,26 +1101,30 @@
       <c r="Q9">
         <v>8</v>
       </c>
-      <c r="R9" t="b">
-        <v>0</v>
+      <c r="R9">
+        <v>0.5</v>
       </c>
       <c r="S9">
-        <v>10800</v>
+        <v>14400</v>
       </c>
       <c r="T9">
-        <f>24*30*6</f>
-        <v>4320</v>
+        <f t="shared" si="3"/>
+        <v>6480</v>
       </c>
       <c r="U9">
-        <f t="shared" si="1"/>
-        <v>192720</v>
+        <f>35*365*24</f>
+        <v>306600</v>
       </c>
       <c r="V9">
         <f t="shared" si="2"/>
         <v>43800</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -1088,20 +1147,20 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="I10">
         <v>7000</v>
       </c>
       <c r="J10">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="K10">
-        <v>240</v>
+        <v>30</v>
       </c>
       <c r="L10">
-        <v>360</v>
+        <v>40</v>
       </c>
       <c r="M10">
         <v>720</v>
@@ -1113,13 +1172,13 @@
         <v>240</v>
       </c>
       <c r="P10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>4</v>
-      </c>
-      <c r="R10" t="b">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>0.75</v>
       </c>
       <c r="S10">
         <v>10800</v>
@@ -1129,12 +1188,1308 @@
         <v>4320</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
-        <v>192720</v>
+        <f>25*365*24</f>
+        <v>219000</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
         <v>43800</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>720</v>
+      </c>
+      <c r="G11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I11">
+        <v>7000</v>
+      </c>
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11">
+        <v>30</v>
+      </c>
+      <c r="L11">
+        <v>40</v>
+      </c>
+      <c r="M11">
+        <v>720</v>
+      </c>
+      <c r="N11">
+        <v>480</v>
+      </c>
+      <c r="O11">
+        <v>240</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>8</v>
+      </c>
+      <c r="R11">
+        <v>0.75</v>
+      </c>
+      <c r="S11">
+        <v>10800</v>
+      </c>
+      <c r="T11">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U11">
+        <f>30*365*24</f>
+        <v>262800</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>720</v>
+      </c>
+      <c r="G12">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I12">
+        <v>7000</v>
+      </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12">
+        <v>30</v>
+      </c>
+      <c r="L12">
+        <v>40</v>
+      </c>
+      <c r="M12">
+        <v>720</v>
+      </c>
+      <c r="N12">
+        <v>480</v>
+      </c>
+      <c r="O12">
+        <v>240</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>8</v>
+      </c>
+      <c r="R12">
+        <v>0.75</v>
+      </c>
+      <c r="S12">
+        <v>10800</v>
+      </c>
+      <c r="T12">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U12">
+        <f>35*365*24</f>
+        <v>306600</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>42</v>
+      </c>
+      <c r="F13">
+        <v>720</v>
+      </c>
+      <c r="G13">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I13">
+        <v>7000</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13">
+        <v>30</v>
+      </c>
+      <c r="L13">
+        <v>40</v>
+      </c>
+      <c r="M13">
+        <v>720</v>
+      </c>
+      <c r="N13">
+        <v>480</v>
+      </c>
+      <c r="O13">
+        <v>240</v>
+      </c>
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>8</v>
+      </c>
+      <c r="R13">
+        <v>0.75</v>
+      </c>
+      <c r="S13">
+        <v>14400</v>
+      </c>
+      <c r="T13">
+        <f>24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U13">
+        <f>25*365*24</f>
+        <v>219000</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <v>720</v>
+      </c>
+      <c r="G14">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I14">
+        <v>7000</v>
+      </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
+      <c r="K14">
+        <v>30</v>
+      </c>
+      <c r="L14">
+        <v>40</v>
+      </c>
+      <c r="M14">
+        <v>720</v>
+      </c>
+      <c r="N14">
+        <v>480</v>
+      </c>
+      <c r="O14">
+        <v>240</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <v>0.75</v>
+      </c>
+      <c r="S14">
+        <v>14400</v>
+      </c>
+      <c r="T14">
+        <f t="shared" ref="T14:T15" si="4">24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U14">
+        <f>30*365*24</f>
+        <v>262800</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>720</v>
+      </c>
+      <c r="G15">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I15">
+        <v>7000</v>
+      </c>
+      <c r="J15">
+        <v>100</v>
+      </c>
+      <c r="K15">
+        <v>30</v>
+      </c>
+      <c r="L15">
+        <v>40</v>
+      </c>
+      <c r="M15">
+        <v>720</v>
+      </c>
+      <c r="N15">
+        <v>480</v>
+      </c>
+      <c r="O15">
+        <v>240</v>
+      </c>
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>8</v>
+      </c>
+      <c r="R15">
+        <v>0.75</v>
+      </c>
+      <c r="S15">
+        <v>14400</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="4"/>
+        <v>6480</v>
+      </c>
+      <c r="U15">
+        <f>35*365*24</f>
+        <v>306600</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="0"/>
+        <v>438000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>720</v>
+      </c>
+      <c r="G16">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I16">
+        <v>7000</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>30</v>
+      </c>
+      <c r="L16">
+        <v>40</v>
+      </c>
+      <c r="M16">
+        <v>720</v>
+      </c>
+      <c r="N16">
+        <v>480</v>
+      </c>
+      <c r="O16">
+        <v>240</v>
+      </c>
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>8</v>
+      </c>
+      <c r="R16">
+        <v>0.5</v>
+      </c>
+      <c r="S16">
+        <v>10800</v>
+      </c>
+      <c r="T16">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U16">
+        <f>25*365*24</f>
+        <v>219000</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ref="W16:W27" si="5">24*365*12</f>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>720</v>
+      </c>
+      <c r="G17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I17">
+        <v>7000</v>
+      </c>
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>30</v>
+      </c>
+      <c r="L17">
+        <v>40</v>
+      </c>
+      <c r="M17">
+        <v>720</v>
+      </c>
+      <c r="N17">
+        <v>480</v>
+      </c>
+      <c r="O17">
+        <v>240</v>
+      </c>
+      <c r="P17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>8</v>
+      </c>
+      <c r="R17">
+        <v>0.5</v>
+      </c>
+      <c r="S17">
+        <v>10800</v>
+      </c>
+      <c r="T17">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U17">
+        <f>30*365*24</f>
+        <v>262800</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>40</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>42</v>
+      </c>
+      <c r="F18">
+        <v>720</v>
+      </c>
+      <c r="G18">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I18">
+        <v>7000</v>
+      </c>
+      <c r="J18">
+        <v>100</v>
+      </c>
+      <c r="K18">
+        <v>30</v>
+      </c>
+      <c r="L18">
+        <v>40</v>
+      </c>
+      <c r="M18">
+        <v>720</v>
+      </c>
+      <c r="N18">
+        <v>480</v>
+      </c>
+      <c r="O18">
+        <v>240</v>
+      </c>
+      <c r="P18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>8</v>
+      </c>
+      <c r="R18">
+        <v>0.5</v>
+      </c>
+      <c r="S18">
+        <v>10800</v>
+      </c>
+      <c r="T18">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U18">
+        <f>35*365*24</f>
+        <v>306600</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <v>720</v>
+      </c>
+      <c r="G19">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I19">
+        <v>7000</v>
+      </c>
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19">
+        <v>30</v>
+      </c>
+      <c r="L19">
+        <v>40</v>
+      </c>
+      <c r="M19">
+        <v>720</v>
+      </c>
+      <c r="N19">
+        <v>480</v>
+      </c>
+      <c r="O19">
+        <v>240</v>
+      </c>
+      <c r="P19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>8</v>
+      </c>
+      <c r="R19">
+        <v>0.5</v>
+      </c>
+      <c r="S19">
+        <v>14400</v>
+      </c>
+      <c r="T19">
+        <f>24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U19">
+        <f>25*365*24</f>
+        <v>219000</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>25</v>
+      </c>
+      <c r="E20">
+        <v>42</v>
+      </c>
+      <c r="F20">
+        <v>720</v>
+      </c>
+      <c r="G20">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I20">
+        <v>7000</v>
+      </c>
+      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="K20">
+        <v>30</v>
+      </c>
+      <c r="L20">
+        <v>40</v>
+      </c>
+      <c r="M20">
+        <v>720</v>
+      </c>
+      <c r="N20">
+        <v>480</v>
+      </c>
+      <c r="O20">
+        <v>240</v>
+      </c>
+      <c r="P20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <v>0.5</v>
+      </c>
+      <c r="S20">
+        <v>14400</v>
+      </c>
+      <c r="T20">
+        <f t="shared" ref="T20:T21" si="6">24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U20">
+        <f>30*365*24</f>
+        <v>262800</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>42</v>
+      </c>
+      <c r="F21">
+        <v>720</v>
+      </c>
+      <c r="G21">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I21">
+        <v>7000</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21">
+        <v>30</v>
+      </c>
+      <c r="L21">
+        <v>40</v>
+      </c>
+      <c r="M21">
+        <v>720</v>
+      </c>
+      <c r="N21">
+        <v>480</v>
+      </c>
+      <c r="O21">
+        <v>240</v>
+      </c>
+      <c r="P21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>8</v>
+      </c>
+      <c r="R21">
+        <v>0.5</v>
+      </c>
+      <c r="S21">
+        <v>14400</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="6"/>
+        <v>6480</v>
+      </c>
+      <c r="U21">
+        <f>35*365*24</f>
+        <v>306600</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>42</v>
+      </c>
+      <c r="F22">
+        <v>720</v>
+      </c>
+      <c r="G22">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I22">
+        <v>7000</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22">
+        <v>30</v>
+      </c>
+      <c r="L22">
+        <v>40</v>
+      </c>
+      <c r="M22">
+        <v>720</v>
+      </c>
+      <c r="N22">
+        <v>480</v>
+      </c>
+      <c r="O22">
+        <v>240</v>
+      </c>
+      <c r="P22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>8</v>
+      </c>
+      <c r="R22">
+        <v>0.75</v>
+      </c>
+      <c r="S22">
+        <v>10800</v>
+      </c>
+      <c r="T22">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U22">
+        <f>25*365*24</f>
+        <v>219000</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>25</v>
+      </c>
+      <c r="E23">
+        <v>42</v>
+      </c>
+      <c r="F23">
+        <v>720</v>
+      </c>
+      <c r="G23">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I23">
+        <v>7000</v>
+      </c>
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23">
+        <v>30</v>
+      </c>
+      <c r="L23">
+        <v>40</v>
+      </c>
+      <c r="M23">
+        <v>720</v>
+      </c>
+      <c r="N23">
+        <v>480</v>
+      </c>
+      <c r="O23">
+        <v>240</v>
+      </c>
+      <c r="P23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>8</v>
+      </c>
+      <c r="R23">
+        <v>0.75</v>
+      </c>
+      <c r="S23">
+        <v>10800</v>
+      </c>
+      <c r="T23">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U23">
+        <f>30*365*24</f>
+        <v>262800</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>42</v>
+      </c>
+      <c r="F24">
+        <v>720</v>
+      </c>
+      <c r="G24">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I24">
+        <v>7000</v>
+      </c>
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24">
+        <v>30</v>
+      </c>
+      <c r="L24">
+        <v>40</v>
+      </c>
+      <c r="M24">
+        <v>720</v>
+      </c>
+      <c r="N24">
+        <v>480</v>
+      </c>
+      <c r="O24">
+        <v>240</v>
+      </c>
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>8</v>
+      </c>
+      <c r="R24">
+        <v>0.75</v>
+      </c>
+      <c r="S24">
+        <v>10800</v>
+      </c>
+      <c r="T24">
+        <f>24*30*6</f>
+        <v>4320</v>
+      </c>
+      <c r="U24">
+        <f>35*365*24</f>
+        <v>306600</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>50</v>
+      </c>
+      <c r="B25">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>42</v>
+      </c>
+      <c r="F25">
+        <v>720</v>
+      </c>
+      <c r="G25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I25">
+        <v>7000</v>
+      </c>
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25">
+        <v>30</v>
+      </c>
+      <c r="L25">
+        <v>40</v>
+      </c>
+      <c r="M25">
+        <v>720</v>
+      </c>
+      <c r="N25">
+        <v>480</v>
+      </c>
+      <c r="O25">
+        <v>240</v>
+      </c>
+      <c r="P25" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>8</v>
+      </c>
+      <c r="R25">
+        <v>0.75</v>
+      </c>
+      <c r="S25">
+        <v>14400</v>
+      </c>
+      <c r="T25">
+        <f>24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U25">
+        <f>25*365*24</f>
+        <v>219000</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>40</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>42</v>
+      </c>
+      <c r="F26">
+        <v>720</v>
+      </c>
+      <c r="G26">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I26">
+        <v>7000</v>
+      </c>
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
+      <c r="L26">
+        <v>40</v>
+      </c>
+      <c r="M26">
+        <v>720</v>
+      </c>
+      <c r="N26">
+        <v>480</v>
+      </c>
+      <c r="O26">
+        <v>240</v>
+      </c>
+      <c r="P26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>8</v>
+      </c>
+      <c r="R26">
+        <v>0.75</v>
+      </c>
+      <c r="S26">
+        <v>14400</v>
+      </c>
+      <c r="T26">
+        <f t="shared" ref="T26:T27" si="7">24*30*9</f>
+        <v>6480</v>
+      </c>
+      <c r="U26">
+        <f>30*365*24</f>
+        <v>262800</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="5"/>
+        <v>105120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>40</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>42</v>
+      </c>
+      <c r="F27">
+        <v>720</v>
+      </c>
+      <c r="G27">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>438000</v>
+      </c>
+      <c r="I27">
+        <v>7000</v>
+      </c>
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27">
+        <v>30</v>
+      </c>
+      <c r="L27">
+        <v>40</v>
+      </c>
+      <c r="M27">
+        <v>720</v>
+      </c>
+      <c r="N27">
+        <v>480</v>
+      </c>
+      <c r="O27">
+        <v>240</v>
+      </c>
+      <c r="P27" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>8</v>
+      </c>
+      <c r="R27">
+        <v>0.75</v>
+      </c>
+      <c r="S27">
+        <v>14400</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="7"/>
+        <v>6480</v>
+      </c>
+      <c r="U27">
+        <f>35*365*24</f>
+        <v>306600</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="5"/>
+        <v>105120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try the runs for record again!
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a35891ba506d4b9/PhD Work/Dissertation/Programming/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="11_525EA6C75FBDEF2E32167C2D13DA69F02BD21A3E" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{5C8BED0A-83DF-4AC5-8B44-3B3AD5F1B57A}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="113_{42DE64B1-7F60-4D78-9CF2-246A376184AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{FACD162D-A5B4-403F-B25B-4FA5F43DA35A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$U$1:$U$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$U$1:$U$13</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,19 +573,19 @@
         <v>10800</v>
       </c>
       <c r="T2">
-        <f>24*30*6</f>
-        <v>4320</v>
+        <f>24*30*12</f>
+        <v>8640</v>
       </c>
       <c r="U2">
-        <f>50*365*24</f>
-        <v>438000</v>
+        <f>100*365*24</f>
+        <v>876000</v>
       </c>
       <c r="V2">
         <f>5*365*24</f>
         <v>43800</v>
       </c>
       <c r="W2">
-        <f t="shared" ref="W2:W8" si="0">50*365*24</f>
+        <f t="shared" ref="W2:W6" si="0">50*365*24</f>
         <v>438000</v>
       </c>
       <c r="X2" t="s">
@@ -652,12 +652,12 @@
         <v>14400</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T4" si="1">24*30*9</f>
+        <f t="shared" ref="T3:T7" si="1">24*30*9</f>
         <v>6480</v>
       </c>
       <c r="U3">
-        <f>50*365*24</f>
-        <v>438000</v>
+        <f t="shared" ref="U3:U8" si="2">100*365*24</f>
+        <v>876000</v>
       </c>
       <c r="V3">
         <f>5*365*24</f>
@@ -731,12 +731,12 @@
         <v>18000</v>
       </c>
       <c r="T4">
-        <f t="shared" si="1"/>
-        <v>6480</v>
+        <f>24*30*12</f>
+        <v>8640</v>
       </c>
       <c r="U4">
-        <f>50*365*24</f>
-        <v>438000</v>
+        <f t="shared" si="2"/>
+        <v>876000</v>
       </c>
       <c r="V4">
         <f>5*365*24</f>
@@ -773,7 +773,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H12" si="2">50*24*365</f>
+        <f t="shared" ref="H5:H8" si="3">50*24*365</f>
         <v>438000</v>
       </c>
       <c r="I5">
@@ -807,18 +807,18 @@
         <v>0.5</v>
       </c>
       <c r="S5">
-        <v>18000</v>
+        <v>14400</v>
       </c>
       <c r="T5">
-        <f>24*30*6</f>
-        <v>4320</v>
+        <f t="shared" si="1"/>
+        <v>6480</v>
       </c>
       <c r="U5">
-        <f>30*365*24</f>
-        <v>262800</v>
+        <f t="shared" si="2"/>
+        <v>876000</v>
       </c>
       <c r="V5">
-        <f t="shared" ref="V5:V12" si="3">5*365*24</f>
+        <f t="shared" ref="V5:V8" si="4">5*365*24</f>
         <v>43800</v>
       </c>
       <c r="W5">
@@ -849,7 +849,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>438000</v>
       </c>
       <c r="I6">
@@ -886,15 +886,15 @@
         <v>18000</v>
       </c>
       <c r="T6">
-        <f>24*30*6</f>
-        <v>4320</v>
+        <f t="shared" ref="T6:T8" si="5">24*30*12</f>
+        <v>8640</v>
       </c>
       <c r="U6">
-        <f>35*365*24</f>
-        <v>306600</v>
+        <f t="shared" si="2"/>
+        <v>876000</v>
       </c>
       <c r="V6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43800</v>
       </c>
       <c r="W6">
@@ -925,7 +925,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>438000</v>
       </c>
       <c r="I7">
@@ -962,20 +962,20 @@
         <v>14400</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:T8" si="4">24*30*9</f>
+        <f t="shared" si="1"/>
         <v>6480</v>
       </c>
       <c r="U7">
-        <f>30*365*24</f>
-        <v>262800</v>
+        <f t="shared" si="2"/>
+        <v>876000</v>
       </c>
       <c r="V7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43800</v>
       </c>
       <c r="W7">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <f t="shared" ref="W7:W8" si="6">24*365*12</f>
+        <v>105120</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1001,7 +1001,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>438000</v>
       </c>
       <c r="I8">
@@ -1035,331 +1035,27 @@
         <v>0.5</v>
       </c>
       <c r="S8">
-        <v>14400</v>
+        <v>18000</v>
       </c>
       <c r="T8">
+        <f t="shared" ref="T8" si="7">24*30*12</f>
+        <v>8640</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>876000</v>
+      </c>
+      <c r="V8">
         <f t="shared" si="4"/>
-        <v>6480</v>
-      </c>
-      <c r="U8">
-        <f>35*365*24</f>
-        <v>306600</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="3"/>
         <v>43800</v>
       </c>
       <c r="W8">
-        <f t="shared" si="0"/>
-        <v>438000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>50</v>
-      </c>
-      <c r="B9">
-        <v>50</v>
-      </c>
-      <c r="C9">
-        <v>40</v>
-      </c>
-      <c r="D9">
-        <v>25</v>
-      </c>
-      <c r="E9">
-        <v>42</v>
-      </c>
-      <c r="F9">
-        <v>720</v>
-      </c>
-      <c r="G9">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>438000</v>
-      </c>
-      <c r="I9">
-        <v>7000</v>
-      </c>
-      <c r="J9">
-        <v>100</v>
-      </c>
-      <c r="K9">
-        <v>30</v>
-      </c>
-      <c r="L9">
-        <v>40</v>
-      </c>
-      <c r="M9">
-        <v>720</v>
-      </c>
-      <c r="N9">
-        <v>480</v>
-      </c>
-      <c r="O9">
-        <v>240</v>
-      </c>
-      <c r="P9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>8</v>
-      </c>
-      <c r="R9">
-        <v>0.5</v>
-      </c>
-      <c r="S9">
-        <v>18000</v>
-      </c>
-      <c r="T9">
-        <f>24*30*6</f>
-        <v>4320</v>
-      </c>
-      <c r="U9">
-        <f>30*365*24</f>
-        <v>262800</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="3"/>
-        <v>43800</v>
-      </c>
-      <c r="W9">
-        <f t="shared" ref="W9:W12" si="5">24*365*12</f>
-        <v>105120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>50</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-      <c r="C10">
-        <v>40</v>
-      </c>
-      <c r="D10">
-        <v>25</v>
-      </c>
-      <c r="E10">
-        <v>42</v>
-      </c>
-      <c r="F10">
-        <v>720</v>
-      </c>
-      <c r="G10">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>438000</v>
-      </c>
-      <c r="I10">
-        <v>7000</v>
-      </c>
-      <c r="J10">
-        <v>100</v>
-      </c>
-      <c r="K10">
-        <v>30</v>
-      </c>
-      <c r="L10">
-        <v>40</v>
-      </c>
-      <c r="M10">
-        <v>720</v>
-      </c>
-      <c r="N10">
-        <v>480</v>
-      </c>
-      <c r="O10">
-        <v>240</v>
-      </c>
-      <c r="P10" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>8</v>
-      </c>
-      <c r="R10">
-        <v>0.5</v>
-      </c>
-      <c r="S10">
-        <v>18000</v>
-      </c>
-      <c r="T10">
-        <f>24*30*6</f>
-        <v>4320</v>
-      </c>
-      <c r="U10">
-        <f>35*365*24</f>
-        <v>306600</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="3"/>
-        <v>43800</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="5"/>
-        <v>105120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>50</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11">
-        <v>40</v>
-      </c>
-      <c r="D11">
-        <v>25</v>
-      </c>
-      <c r="E11">
-        <v>42</v>
-      </c>
-      <c r="F11">
-        <v>720</v>
-      </c>
-      <c r="G11">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>438000</v>
-      </c>
-      <c r="I11">
-        <v>7000</v>
-      </c>
-      <c r="J11">
-        <v>100</v>
-      </c>
-      <c r="K11">
-        <v>30</v>
-      </c>
-      <c r="L11">
-        <v>40</v>
-      </c>
-      <c r="M11">
-        <v>720</v>
-      </c>
-      <c r="N11">
-        <v>480</v>
-      </c>
-      <c r="O11">
-        <v>240</v>
-      </c>
-      <c r="P11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>8</v>
-      </c>
-      <c r="R11">
-        <v>0.5</v>
-      </c>
-      <c r="S11">
-        <v>14400</v>
-      </c>
-      <c r="T11">
-        <f t="shared" ref="T11:T12" si="6">24*30*9</f>
-        <v>6480</v>
-      </c>
-      <c r="U11">
-        <f>30*365*24</f>
-        <v>262800</v>
-      </c>
-      <c r="V11">
-        <f t="shared" si="3"/>
-        <v>43800</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="5"/>
-        <v>105120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>25</v>
-      </c>
-      <c r="E12">
-        <v>42</v>
-      </c>
-      <c r="F12">
-        <v>720</v>
-      </c>
-      <c r="G12">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>438000</v>
-      </c>
-      <c r="I12">
-        <v>7000</v>
-      </c>
-      <c r="J12">
-        <v>100</v>
-      </c>
-      <c r="K12">
-        <v>30</v>
-      </c>
-      <c r="L12">
-        <v>40</v>
-      </c>
-      <c r="M12">
-        <v>720</v>
-      </c>
-      <c r="N12">
-        <v>480</v>
-      </c>
-      <c r="O12">
-        <v>240</v>
-      </c>
-      <c r="P12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>8</v>
-      </c>
-      <c r="R12">
-        <v>0.5</v>
-      </c>
-      <c r="S12">
-        <v>14400</v>
-      </c>
-      <c r="T12">
         <f t="shared" si="6"/>
-        <v>6480</v>
-      </c>
-      <c r="U12">
-        <f>35*365*24</f>
-        <v>306600</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="3"/>
-        <v>43800</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="5"/>
         <v>105120</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="U1:U16" xr:uid="{7D391075-279E-48EA-AF93-D89D1BAA50CC}"/>
+  <autoFilter ref="U1:U13" xr:uid="{7D391075-279E-48EA-AF93-D89D1BAA50CC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed the no stagger options. Remember, you can go back and run more of it, but this shows it to be a non-starter. You can discuss this.
</commit_message>
<xml_diff>
--- a/FleetResParam.xlsx
+++ b/FleetResParam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a35891ba506d4b9/PhD Work/Dissertation/Programming/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="113_{42DE64B1-7F60-4D78-9CF2-246A376184AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{FACD162D-A5B4-403F-B25B-4FA5F43DA35A}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="113_{42DE64B1-7F60-4D78-9CF2-246A376184AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{407F99F2-6451-45AB-8F0D-FA931A466FB7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>NUM_AIRCRAFT</t>
   </si>
@@ -110,7 +110,7 @@
     <t>Base case no SLEP</t>
   </si>
   <si>
-    <t>Base SLEP case with no stagger</t>
+    <t>Base case no SLEP with surge</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
@@ -585,7 +585,7 @@
         <v>43800</v>
       </c>
       <c r="W2">
-        <f t="shared" ref="W2:W6" si="0">50*365*24</f>
+        <f t="shared" ref="W2:W4" si="0">50*365*24</f>
         <v>438000</v>
       </c>
       <c r="X2" t="s">
@@ -615,7 +615,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H3">
-        <f>50*24*365</f>
+        <f t="shared" ref="H3:H7" si="1">50*24*365</f>
         <v>438000</v>
       </c>
       <c r="I3">
@@ -646,30 +646,27 @@
         <v>8</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S3">
         <v>14400</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T7" si="1">24*30*9</f>
+        <f t="shared" ref="T3:T6" si="2">24*30*9</f>
         <v>6480</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U8" si="2">100*365*24</f>
+        <f t="shared" ref="U3:U7" si="3">100*365*24</f>
         <v>876000</v>
       </c>
       <c r="V3">
-        <f>5*365*24</f>
+        <f t="shared" ref="V3:V7" si="4">5*365*24</f>
         <v>43800</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
         <v>438000</v>
       </c>
-      <c r="X3" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -694,7 +691,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H4">
-        <f>50*24*365</f>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="I4">
@@ -725,30 +722,27 @@
         <v>8</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S4">
         <v>18000</v>
       </c>
       <c r="T4">
-        <f>24*30*12</f>
+        <f t="shared" ref="T4" si="5">24*30*12</f>
         <v>8640</v>
       </c>
       <c r="U4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>876000</v>
       </c>
       <c r="V4">
-        <f>5*365*24</f>
+        <f t="shared" si="4"/>
         <v>43800</v>
       </c>
       <c r="W4">
         <f t="shared" si="0"/>
         <v>438000</v>
       </c>
-      <c r="X4" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -773,7 +767,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H8" si="3">50*24*365</f>
+        <f>50*24*365</f>
         <v>438000</v>
       </c>
       <c r="I5">
@@ -798,32 +792,35 @@
         <v>240</v>
       </c>
       <c r="P5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5">
         <v>8</v>
       </c>
       <c r="R5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>14400</v>
+        <v>10800</v>
       </c>
       <c r="T5">
-        <f t="shared" si="1"/>
-        <v>6480</v>
+        <f>24*30*12</f>
+        <v>8640</v>
       </c>
       <c r="U5">
-        <f t="shared" si="2"/>
+        <f>100*365*24</f>
         <v>876000</v>
       </c>
       <c r="V5">
-        <f t="shared" ref="V5:V8" si="4">5*365*24</f>
+        <f>5*365*24</f>
         <v>43800</v>
       </c>
       <c r="W5">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <f t="shared" ref="W5" si="6">24*365*12</f>
+        <v>105120</v>
+      </c>
+      <c r="X5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -849,7 +846,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="I6">
@@ -883,14 +880,14 @@
         <v>0.5</v>
       </c>
       <c r="S6">
-        <v>18000</v>
+        <v>14400</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:T8" si="5">24*30*12</f>
-        <v>8640</v>
+        <f t="shared" si="2"/>
+        <v>6480</v>
       </c>
       <c r="U6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>876000</v>
       </c>
       <c r="V6">
@@ -898,8 +895,8 @@
         <v>43800</v>
       </c>
       <c r="W6">
-        <f t="shared" si="0"/>
-        <v>438000</v>
+        <f t="shared" ref="W6:W7" si="7">24*365*12</f>
+        <v>105120</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -925,7 +922,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>438000</v>
       </c>
       <c r="I7">
@@ -959,14 +956,14 @@
         <v>0.5</v>
       </c>
       <c r="S7">
-        <v>14400</v>
+        <v>18000</v>
       </c>
       <c r="T7">
-        <f t="shared" si="1"/>
-        <v>6480</v>
+        <f t="shared" ref="T7" si="8">24*30*12</f>
+        <v>8640</v>
       </c>
       <c r="U7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>876000</v>
       </c>
       <c r="V7">
@@ -974,83 +971,7 @@
         <v>43800</v>
       </c>
       <c r="W7">
-        <f t="shared" ref="W7:W8" si="6">24*365*12</f>
-        <v>105120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>50</v>
-      </c>
-      <c r="B8">
-        <v>50</v>
-      </c>
-      <c r="C8">
-        <v>40</v>
-      </c>
-      <c r="D8">
-        <v>25</v>
-      </c>
-      <c r="E8">
-        <v>42</v>
-      </c>
-      <c r="F8">
-        <v>720</v>
-      </c>
-      <c r="G8">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="3"/>
-        <v>438000</v>
-      </c>
-      <c r="I8">
-        <v>7000</v>
-      </c>
-      <c r="J8">
-        <v>100</v>
-      </c>
-      <c r="K8">
-        <v>30</v>
-      </c>
-      <c r="L8">
-        <v>40</v>
-      </c>
-      <c r="M8">
-        <v>720</v>
-      </c>
-      <c r="N8">
-        <v>480</v>
-      </c>
-      <c r="O8">
-        <v>240</v>
-      </c>
-      <c r="P8" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>8</v>
-      </c>
-      <c r="R8">
-        <v>0.5</v>
-      </c>
-      <c r="S8">
-        <v>18000</v>
-      </c>
-      <c r="T8">
-        <f t="shared" ref="T8" si="7">24*30*12</f>
-        <v>8640</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="2"/>
-        <v>876000</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="4"/>
-        <v>43800</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>105120</v>
       </c>
     </row>

</xml_diff>